<commit_message>
util file xltojson.py added
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -11,15 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="349">
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Title_link</t>
-  </si>
-  <si>
-    <t>Headline</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="296">
+  <si>
+    <t>title</t>
   </si>
   <si>
     <t>description</t>
@@ -40,19 +34,16 @@
     <t>cuisine</t>
   </si>
   <si>
-    <t>Dish Type</t>
+    <t>dishtype</t>
   </si>
   <si>
     <t>mark</t>
   </si>
   <si>
-    <t>Meal Type</t>
+    <t>mealtype</t>
   </si>
   <si>
     <t>Asian Beef with Snow Peas</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/15679/asian-beef-with-snow-peas/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
   </si>
   <si>
     <t>"Stir-fried beef in a light gingery sauce. Serve over steamed rice or hot egg noodles."</t>
@@ -86,9 +77,6 @@
     <t>Asian Fire Meat</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/37965/asian-fire-meat/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 35</t>
-  </si>
-  <si>
     <t>"For a great tasting beef dish from Asia, fire meat is delicious and easy to prepare. Ice cold beer is the beverage recommended with fire meat."</t>
   </si>
   <si>
@@ -111,16 +99,13 @@
     <t>Beef Egg Rolls</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/18252/beef-egg-rolls/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 46</t>
-  </si>
-  <si>
     <t>"Crispy fried egg rolls stuffed with ground beef, cabbage, and delicious seasonings. A personal creation of mine that goes well with any Chinese dish. The sherry makes it better."</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/250x250/195107.jpg,https://images.media-allrecipes.com/userphotos/125x70/195107.jpg</t>
   </si>
   <si>
-    <t>1 pound-ground beef,lean; 1-onion flake,; 1/2 teaspoon-garlic,dried minced ; 2 tablespoons-soy sauce; 1/2 teaspoon-salt; 1/2 teaspoon-peppercorn,ground; 2 tablespoons-sherry; 1 teaspoon-ground ginger,; 1-cabbage,large headed, finely shredded; 1/4 cup-water; 1 tablespoon-vegetable oil; 1 teaspoon-sugar; 2 tablespoons-soy sauce; 2 tablespoons-sherry; 1/2 teaspoon-salt; 1/2 teaspoon-peppercorn,ground; 2 quarts-vegetable oil; 1 (16 ounce) package-egg,to make egg-roll wrappers</t>
+    <t>1 pound-ground beef,lean; 1-onion flake,; 1/2 teaspoon-garlic,dried minced ; 2 tablespoons-soy sauce; 1/2 teaspoon-salt; 1/2 teaspoon-peppercorn,ground; 2 tablespoons-sherry; 1 teaspoon-ground ginger,; 1-cabbage,large headed, finely shredded; 1/4 cup-water; 1 tablespoon-vegetable oil; 1 teaspoon-sugar; 2 tablespoons-soy sauce; 2 tablespoons-sherry; 1/2 teaspoon-salt; 1/2 teaspoon-peppercorn,ground; 2 quarts-vegetable oil; 1 (16 ounce) package-egg,to make egg roll wrappers</t>
   </si>
   <si>
     <t>45 m</t>
@@ -134,13 +119,10 @@
  Pour oil into a deep pan and heat to 350 degrees F (175 degrees C). Fill each egg roll wrapper with approximately 1/4 cup of filling and roll up according to package directions. Fry in preheated oil until golden brown. Drain on paper towels and serve hot.</t>
   </si>
   <si>
-    <t>Appetizers and Snacks</t>
+    <t>Appetizers &amp; Snacks</t>
   </si>
   <si>
     <t>Beef Lo Mein</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/231381/beef-lo-mein/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 61</t>
   </si>
   <si>
     <t>"I couldn't find a good lo mein recipe on here, so I'm posting mine. I made it this week and my roommate and I agreed that it was possibly the best that we've ever had."</t>
@@ -166,9 +148,6 @@
     <t>Beefy Chinese Dumplings</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/87535/beefy-chinese-dumplings/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 89</t>
-  </si>
-  <si>
     <t>"This is a delicious meat and veggie dumpling recipe that my mom has been making ever since I can remember. It may take some time and practice when it comes to making these, but it's well worth it. Just boil them in water, and serve hot with soy sauce, or add them to a soup."</t>
   </si>
   <si>
@@ -192,9 +171,6 @@
     <t>Black Pepper Beef and Cabbage Stir Fry</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/50233/black-pepper-beef-and-cabbage-stir-fry/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"A very simple Chinese stir-fry dish which is fabulous in taste. I saw my husband going for two additional servings of it and I had to remind him to leave some for the rest of the family! Serve with hot steamed rice."</t>
   </si>
   <si>
@@ -217,9 +193,6 @@
     <t>Chi Tan T'ang (Egg Drop Soup)</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/12947/chi-tan-tang-egg-drop-soup/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 53</t>
-  </si>
-  <si>
     <t>"The best egg drop soup I've ever had!!! Reheats well in microwave."</t>
   </si>
   <si>
@@ -238,13 +211,10 @@
  In a large saucepan, dissolve bouillon in hot water. Mix cornstarch with a small amount of water, and stir into bouillon. Add soy sauce, vinegar, and green onion. Bring to a boil, then simmer, stirring occasionally. Gradually pour the beaten eggs into the saucepan while stirring. Serve at once.</t>
   </si>
   <si>
-    <t>Soups, Stews and Chili</t>
+    <t>Soups, Stews, and Chili</t>
   </si>
   <si>
     <t>Chinese Cabbage Salad II</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/14447/chinese-cabbage-salad-ii/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 81</t>
   </si>
   <si>
     <t>"This is a wonderful and crunchy cabbage salad with great texture and color.  You can vary the flavor a little by using beef flavored ramen, if you like."</t>
@@ -268,9 +238,6 @@
   </si>
   <si>
     <t>Chinese Fried Noodles</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/34668/chinese-fried-noodles/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 42</t>
   </si>
   <si>
     <t>"This is a quick, easy, and delicious recipe that all will enjoy. Try adding cooked, cubed pork or chicken, bean sprouts, water chestnuts, sliced almonds, or any of your favorite vegetables for versatility."</t>
@@ -294,13 +261,10 @@
     <t>Side Dish</t>
   </si>
   <si>
-    <t>brown</t>
+    <t>yellow</t>
   </si>
   <si>
     <t>Chinese Green Bean Stir-Fry</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/49350/chinese-green-bean-stir-fry/?internalSource=staff pick&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
   </si>
   <si>
     <t>"Asian-style green beans with lots of flavor! This recipe is made for a large party; but can be scaled down for a family dinner.  Serve cold or warm."</t>
@@ -324,16 +288,13 @@
     <t>Chinese Pepper Steak</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/172704/chinese-pepper-steak/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"A delicious meal, served with boiled white rice, that's easy and made from items that I've already got in my cupboards! My mother clipped this recipe from somewhere and it became a specialty of mine; however, I've been unable to find the original source."</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/125x70/7127114.jpg</t>
   </si>
   <si>
-    <t>1 pound-beef sirloin,steaked; 1/4 cup-soy sauce; 2 tablespoons-sugar; 2 tablespoons-cornstarch; 1/2 teaspoon-ground ginger,; 3 tablespoons-vegetable oil, divided; 1-red onion, cut into 1; 1-bell pepper,green,cut into 1-inch squares; 2-tomato, cut into wedges</t>
+    <t>1 pound-beef sirloin,steaked; 1/4 cup-soy sauce; 2 tablespoons-sugar; 2 tablespoons-cornstarch; 1/2 teaspoon-ground ginger,; 3 tablespoons-vegetable oil, divided; 1-red onion, cut into 1; 1-bell pepper,green,cut into 1 inch squares; 2-tomato, cut into wedges</t>
   </si>
   <si>
     <t>Prep15 m
@@ -348,16 +309,13 @@
     <t>Chinese Steamed Buns</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/7011/chinese-steamed-buns/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 45</t>
-  </si>
-  <si>
     <t>"Here's some yummy, Chinese dim sum you can make, either plain without meat fillings, or with meat fillings. A wok equipped with a stainless steel steam plate, a plate with holes to allow steam to pass, is required to make these tasty buns. You may use milk in place of the warm water if you wish."</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/560x315/1121464.jpg,https://images.media-allrecipes.com/userphotos/125x70/1121464.jpg</t>
   </si>
   <si>
-    <t>1 tablespoon-yeast,active,dry; 1 teaspoon-sugar; 1/4 cup-all purpose flour; 1/4 cup-water; 1/2 cup-water,warm; 1/2 cup; all purpose flour; 1/4 teaspoon-salt; 2 tablespoons-sugar; 1 tablespoon-vegetable oil; 1/2 teaspoon-baking powder</t>
+    <t>1 tablespoon-yeast,active,dry; 1 teaspoon-sugar; 1/4 cup-all purpose flour; 1/4 cup-water; 1/2 cup-water,warm; 1/2 cup-all purpose flour; 1/4 teaspoon-salt; 2 tablespoons-sugar; 1 tablespoon-vegetable oil; 1/2 teaspoon-baking powder</t>
   </si>
   <si>
     <t>4 h</t>
@@ -373,13 +331,10 @@
 REMOVE LID BEFORE you turn off heat, or else water will drip back onto bun surface and produce yellowish "blisters" on bun surfaces. Continue steaming batches of buns until all are cooked.</t>
   </si>
   <si>
-    <t>Bread</t>
+    <t>Bread Recipes</t>
   </si>
   <si>
     <t>Chinese Style Sesame Sauce</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/46908/chinese-style-sesame-sauce/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 59</t>
   </si>
   <si>
     <t>"This is the SAUCE for Chinese restaurant style sesame chicken and broccoli. This sauce can be poured over fried chicken, or used as a dipping sauce for fried chicken. I emphasize not using too much vinegar because it turns into a sweet-n-sour type sauce. But you do need a 'touch' of vinegar."</t>
@@ -398,9 +353,6 @@
   </si>
   <si>
     <t>Chinese-Style Baby Bok Choy with Mushroom Sauce</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/215795/chinese-style-baby-bok-choy-with-mushroom-sauce/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 67</t>
   </si>
   <si>
     <t>"This is a delicious dish. It is an authentic Chinese recipe that I use for my cooking. Baby bok choy and mushroom are the two main ingredients. "</t>
@@ -421,9 +373,6 @@
   </si>
   <si>
     <t>Crab Rangoon I</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/14850/crab-rangoon-i/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 60</t>
   </si>
   <si>
     <t>"Everyone will love these bite-size, fried dumplings stuffed with crab. You can make these in advance of the festivities, and freeze on trays until party time."</t>
@@ -447,16 +396,13 @@
     <t>Crispy Ginger Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/237807/crispy-ginger-beef/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 73</t>
-  </si>
-  <si>
     <t>"This recipe is so much better than take out! Serve it with homemade fried rice or plain rice. If you like spicy, just add more chili pepper flakes!"</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/560x315/5307100.jpg,https://images.media-allrecipes.com/userphotos/125x70/5307100.jpg</t>
   </si>
   <si>
-    <t>3/4 cup-cornstarch; 1/2 cup-water; 2-egg; 1 pound-beef steak,flank,cut into thin strips; 1/2 cup-canola oil,; 1-carrot, large,cut into matchstick; 1-bell pepper,green,cut into matchstick-size pieces; 1-bell pepper,red,cut into matchstick-size pieces; 3-scallion, chopped; 1/4 cup-ginger, minced fresh; 5 cloves-garlic, minced; 1/2 cup-sugar; 1/4 cup-rice vinegar; 3 tablespoons-soy sauce; 1 tablespoon-sesame oil; 1 tablespoon or to taste-red pepper flake,</t>
+    <t>3/4 cup-cornstarch; 1/2 cup-water; 2-egg; 1 pound-beef steak,flank,cut into thin strips; 1/2 cup-canola oil,; 1-carrot, large,cut into matchstick; 1-bell pepper,green,cut into matchstick size pieces; 1-bell pepper,red,cut into matchstick size pieces; 3-scallion, chopped; 1/4 cup-ginger, minced fresh; 5 cloves-garlic, minced; 1/2 cup-sugar; 1/4 cup-rice vinegar; 3 tablespoons-soy sauce; 1 tablespoon-sesame oil; 1 tablespoon or to taste-red pepper flake,</t>
   </si>
   <si>
     <t>Prep25 m
@@ -471,9 +417,6 @@
     <t>Crispy Orange Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/57966/crispy-orange-beef/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"A delicious crispy and sweet, yet mildly spiced beef stir-fry recipe. Great served with steamed rice and broccoli."</t>
   </si>
   <si>
@@ -498,9 +441,6 @@
     <t>Easy Chinese Corn Soup</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/29704/easy-chinese-corn-soup/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 86</t>
-  </si>
-  <si>
     <t>"This quick and easy soup is so good that I never bother ordering it from Chinese restaurants anymore!"</t>
   </si>
   <si>
@@ -519,9 +459,6 @@
     <t>Egg Drop Soup (Better than Restaurant Quality!)</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/115965/egg-drop-soup-better-than-restaurant-quality/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"After many many trips to different Chinese restaurants looking for a good bowl of egg drop soup, I decided to take it upon myself to create what I feel is the ultimate in egg drop soup. I hope you enjoy it as much as I do!"</t>
   </si>
   <si>
@@ -543,9 +480,6 @@
     <t>Egg Drop Soup I</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/13207/egg-drop-soup-i/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 58</t>
-  </si>
-  <si>
     <t>"A family favorite when we're sick.  Garnish with parsley flakes and serve with soy sauce.  Better than chicken soup!"</t>
   </si>
   <si>
@@ -566,9 +500,6 @@
     <t>Egg Drop Soup II</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/13343/egg-drop-soup-ii/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 39</t>
-  </si>
-  <si>
     <t>"This is a quick and easy recipe that tastes really good.  To add a little more to this soup add one small (7 to 8 ounce) can creamed corn and omit the egg."</t>
   </si>
   <si>
@@ -585,16 +516,13 @@
     <t>Eggplant with Garlic Sauce</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/201964/eggplant-with-garlic-sauce/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 38</t>
-  </si>
-  <si>
     <t>"A mildly spicy (or very spicy if you like) eggplant dish. My mother has been making this for me since I was a child. It is SO GOOD!!"</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/560x315/416924.jpg,https://images.media-allrecipes.com/userphotos/125x70/416924.jpg</t>
   </si>
   <si>
-    <t>3 tablespoons-canola oil; 4-eggplant,chinese,halved lengthwise and cut into 1-inch half moons; 1 cup-water; 1 tablespoon-red pepper flake,crushed; 3 tablespoons-garlic powder; 5 teaspoons-sugar; 1 teaspoon-cornstarch; 2 tablespoons-soy sauce,light; 2 tablespoons-oyster sauce</t>
+    <t>3 tablespoons-canola oil; 4-eggplant,chinese,halved lengthwise and cut into 1 inch half moons; 1 cup-water; 1 tablespoon-red pepper flake,crushed; 3 tablespoons-garlic powder; 5 teaspoons-sugar; 1 teaspoon-cornstarch; 2 tablespoons-soy sauce,light; 2 tablespoons-oyster sauce</t>
   </si>
   <si>
     <t>25 m</t>
@@ -607,9 +535,6 @@
   </si>
   <si>
     <t>Flavorful Beef Stir-Fry</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/223389/flavorful-beef-stir-fry/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 64</t>
   </si>
   <si>
     <t>"A beef stir-fry that has wonderful flavors without using a ton of spices. Fresh ginger mixes will with the soy sauce and makes a quick and easy sauce. Lots of veggies add color and crunch."</t>
@@ -636,9 +561,6 @@
     <t>Honey Walnut Shrimp</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/93234/honey-walnut-shrimp/?internalSource=staff pick&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"Hong Kong Style Chinese recipe! Crispy battered shrimp tossed in creamy sauce topped with sugar coated walnuts"</t>
   </si>
   <si>
@@ -659,9 +581,6 @@
     <t>Hot and Sour Chinese Eggplant</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/52925/hot-and-sour-chinese-eggplant/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 30</t>
-  </si>
-  <si>
     <t>"Eggplant is sauteed, then coated in a spicy sweet sauce. It is simple and delicious! I'm sure you'll enjoy this!"</t>
   </si>
   <si>
@@ -682,9 +601,6 @@
     <t>Hot and Tangy Broccoli Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/86410/hot-and-tangy-broccoli-beef/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 61</t>
-  </si>
-  <si>
     <t>"Tangy and spicy beef and broccoli are a winning combination in this quick stir-fry dinner."</t>
   </si>
   <si>
@@ -708,16 +624,13 @@
     <t>Kikkoman Chinese Pepper Steak</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/86407/kikkoman-chinese-pepper-steak/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 93</t>
-  </si>
-  <si>
     <t>"Beef strips are stir-fried with onion and peppers in this quick stove-top meal. Serve with your favorite rice or noodles."</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/560x315/6293324.jpg,https://images.media-allrecipes.com/userphotos/125x70/6293324.jpg</t>
   </si>
   <si>
-    <t>1 pound-beef steak,sirloin or round,boneless; 1 tablespoon-hoisin sauce,kikkoman preferably; 2 tablespoons-vegetable oil,divided; 2-bell pepper,medium, cut into 1; 2-onion,medium,cut into 1; 1/4 cup-hoisin sauce,kikkoman preferably</t>
+    <t>1 pound-beef steak,sirloin or round,boneless; 1 tablespoon-hoisin sauce,kikkoman preferably; 2 tablespoons-vegetable oil,divided; 2-bell pepper,medium, cut into 1 inch pieces; 2-onion,medium,cut into 1; 1/4 cup-hoisin sauce,kikkoman preferably</t>
   </si>
   <si>
     <t>Cut steak across grain into thin strips, then into 1-inch squares; coat with 1 Tbsp. hoisin sauce.
@@ -726,9 +639,6 @@
   </si>
   <si>
     <t>Mongolian Beef and Spring Onions</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/201849/mongolian-beef-and-spring-onions/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
   </si>
   <si>
     <t>"A soy-based Chinese-style beef dish. Best served over soft rice noodles or rice."</t>
@@ -753,9 +663,6 @@
     <t>Mongolian Beef I</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/22625/mongolian-beef-i/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 33</t>
-  </si>
-  <si>
     <t>"A simple but spicy dish with beef, carrots and green onions. Serve over rice for a very filling meal."</t>
   </si>
   <si>
@@ -777,9 +684,6 @@
     <t>Mongolian Beef II</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/26627/mongolian-beef-ii/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 62</t>
-  </si>
-  <si>
     <t>"Savory strips of sirloin roast are soaked in a spicy marinade and sauteed with green onions. Serve over steamed rice or fried rice noodles."</t>
   </si>
   <si>
@@ -802,9 +706,6 @@
   </si>
   <si>
     <t>Pan-Fried Chinese Pancakes</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/214564/pan-fried-chinese-pancakes/?internalSource=staff pick&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
   </si>
   <si>
     <t>"A delicious brunch snack that can be found in many Chinese breakfast shops.  Its various names include 'cong you bing,' 'jiu cai bing,', 'scallion pancakes,' 'green onion pancakes,' etc.  This particular recipe is passed down through my mother's family, and brings back many good, yummy memories! Can serve with hot-sour sauce, or your favorite Chinese sauce."</t>
@@ -829,9 +730,6 @@
     <t>Peking Duck</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/31972/peking-duck/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 78</t>
-  </si>
-  <si>
     <t>"I have made this recipe and it is delicious. It can be served with plum sauce as well as a fruit sauce. This is actually a short-cut version but it is fantastic."</t>
   </si>
   <si>
@@ -857,9 +755,6 @@
     <t>Pineapple Fried Rice II</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/56140/pineapple-fried-rice-ii/?internalSource=rotd&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"Exotic flavors blend together to create this crowd-pleasing favorite. Contains pineapple, ham, peas, green onion and eggs."</t>
   </si>
   <si>
@@ -880,9 +775,6 @@
     <t>Potstickers (Chinese Dumplings)</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/202975/potstickers-chinese-dumplings/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 91</t>
-  </si>
-  <si>
     <t>"An authentic potsticker recipe using ground beef and ground shrimp instead of the usual pork filling. You can fill the whole package of gyoza wrappers and have filling left over for next time around."</t>
   </si>
   <si>
@@ -906,16 +798,13 @@
     <t>Quick Beef Stir-Fry</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/228823/quick-beef-stir-fry/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 29</t>
-  </si>
-  <si>
     <t>"Quick and easy. I make this on my busiest weeknights."</t>
   </si>
   <si>
     <t>https://images.media-allrecipes.com/userphotos/125x70/6263320.jpg</t>
   </si>
   <si>
-    <t>2 tablespoons-vegetable oil; 1 pound-beef sirloin,cut into 2-inch strips; 1 1/2 cups-broccoli,fresh florets; 1-bell pepper,red, cut into matchsticks; 2-carrot, thinly sliced; 1-scallion, chopped; 1 teaspoon-garlic,minced; 2 tablespoons-soy sauce; 2 tablespoons-sesame seed, toasted</t>
+    <t>2 tablespoons-vegetable oil; 1 pound-beef sirloin,cut into 2 inch strips; 1 1/2 cups-broccoli,fresh florets; 1-bell pepper,red, cut into matchsticks; 2-carrot, thinly sliced; 1-scallion, chopped; 1 teaspoon-garlic,minced; 2 tablespoons-soy sauce; 2 tablespoons-sesame seed, toasted</t>
   </si>
   <si>
     <t>Prep15 m
@@ -928,9 +817,6 @@
     <t>Quick Chinese-Style Vermicelli (Rice Noodles)</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/41761/quick-chinese-style-vermicelli-rice-noodles/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 57</t>
-  </si>
-  <si>
     <t>"Quick and delicious Chinese-style rice noodles."</t>
   </si>
   <si>
@@ -953,9 +839,6 @@
     <t>Restaurant Style Egg Drop Soup</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/45515/restaurant-style-egg-drop-soup/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"This Egg Drop soup is born from a love of the soup and MANY trips to my favorite Chinese restaurant (asking them many questions) resulting in this variation. Compare it to your local restaurant...The simplicity is the key. Soup can be re-heated or frozen and re-heated."</t>
   </si>
   <si>
@@ -975,9 +858,6 @@
     <t>Slow Cooker Mongolian Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/195083/slow-cooker-mongolian-beef/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"I got this recipe from a friend and it is wonderful.  My kids love it.  It tastes like you got it at a Chinese restaurant and the slow cooker does most of the work! Serve over steamed rice."</t>
   </si>
   <si>
@@ -998,9 +878,6 @@
   </si>
   <si>
     <t>Spicy Crispy Beef</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/23420/spicy-crispy-beef/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 42</t>
   </si>
   <si>
     <t>"I've never found a recipe for crispy ginger beef like the ones in the restaurants. I have experimented, and found something pretty close. Serve with rice and some steamed veggies."</t>
@@ -1023,9 +900,6 @@
   </si>
   <si>
     <t>Spicy Orange Zest Beef</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/221127/spicy-orange-zest-beef/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 70</t>
   </si>
   <si>
     <t>"This spicy orange zest beef recipe is not supposed to be Chinese food, or even Americanized Chinese take-out food. It is a lower-fat alternative while still a quick, easy, and surprisingly flavorful meal."</t>
@@ -1055,9 +929,6 @@
     <t>Steamed Fish with Ginger</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/140570/steamed-fish-with-ginger/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 74</t>
-  </si>
-  <si>
     <t>"If you like fish or even anything about Chinese food you'll love this recipe."</t>
   </si>
   <si>
@@ -1079,9 +950,6 @@
     <t>Super-Simple, Super-Spicy Mongolian Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/148831/super-simple-super-spicy-mongolian-beef/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"This is a great-tasting recipe that is easy to prepare ahead and takes minutes to actually cook it! Serve with rice and veggie side for a nice family dinner!"</t>
   </si>
   <si>
@@ -1102,9 +970,6 @@
   </si>
   <si>
     <t>Sweet and Sour Pork Tenderloin</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/222342/sweet-and-sour-pork-tenderloin/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 37</t>
   </si>
   <si>
     <t>"I thoroughly enjoyed this plate of florescent food, and if you're a fan of the Chinese take-out version, I believe you will enjoy this too."</t>
@@ -1133,9 +998,6 @@
     <t>Szechuan Beef</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/20095/szechuan-beef/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 48</t>
-  </si>
-  <si>
     <t>"It is spicy! Serve with rice."</t>
   </si>
   <si>
@@ -1155,9 +1017,6 @@
     <t>Szechwan Shrimp</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/86230/szechwan-shrimp/?internalSource=hub recipe&amp;referringId=695&amp;referringContentType=Recipe Hub</t>
-  </si>
-  <si>
     <t>"Don't let some of the ingredients fool you--this spicy shrimp makes a simple, impressive dish, which I usually make for company. For more or less heat, adjust amount of red pepper. Serve over hot steamed rice."</t>
   </si>
   <si>
@@ -1175,9 +1034,6 @@
   </si>
   <si>
     <t>Vegetable Lo Mein</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/11747/vegetable-lo-mein/?internalSource=recipe hub&amp;referringId=695&amp;referringContentType=Recipe Hub&amp;clickId=cardslot 43</t>
   </si>
   <si>
     <t>"A great accompaniment to any Asian meal. Try adding 3/4 pound cooked meat for variety."</t>
@@ -1200,9 +1056,6 @@
     <t>Besan (Gram Flour) Halwa</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/210476/besan-gram-flour-halwa/?internalSource=streams&amp;referringId=1879&amp;referringContentType=Recipe%20Hub&amp;clickId=st_trending_s</t>
-  </si>
-  <si>
     <t>"If you like the flavour of besan (chickpea flour) in sweets, you will love this halwa. I often make this halwa instead of 'Besan Ladoo' or 'Mysore Pak.' My kids gobble it up even before it has a chance to cool down."</t>
   </si>
   <si>
@@ -1222,16 +1075,10 @@
     <t>Indian</t>
   </si>
   <si>
-    <t>Veg</t>
-  </si>
-  <si>
     <t>Desserts</t>
   </si>
   <si>
     <t>Kulfi</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/19834/kulfi/?internalSource=streams&amp;referringId=1879&amp;referringContentType=Recipe%20Hub&amp;clickId=st_trending_s</t>
   </si>
   <si>
     <t>"This is a simple but delicious recipe for Kulfi (Indian Ice Cream) that I got from my sister-in-law. I have made this several times, and it always gets rave reviews - even the kids love it! For extra flavor, you could add a few drops of rose water or ground pistachios."</t>
@@ -1253,9 +1100,6 @@
   </si>
   <si>
     <t>Shahi Tukra (Indian Bread Pudding)</t>
-  </si>
-  <si>
-    <t>https://www.allrecipes.com/recipe/212813/shahi-tukra-indian-bread-pudding/?internalSource=streams&amp;referringId=1879&amp;referringContentType=Recipe%20Hub&amp;clickId=st_trending_s</t>
   </si>
   <si>
     <t>"This is a very famous Hyderabadi dish and is a very simple, but rich dessert. It is great for a large dinner party as the recipe can be easily multiplied to make more. It is best eaten chilled. If available, you can add a few drops of Kewra essence to the milk mixture once it has cooled."</t>
@@ -1281,9 +1125,6 @@
     <t>Besan Laddu</t>
   </si>
   <si>
-    <t>https://www.allrecipes.com/recipe/167060/besan-laddu/?internalSource=staff%20pick&amp;referringId=1879&amp;referringContentType=Recipe%20Hub</t>
-  </si>
-  <si>
     <t>"A delicious Indian sweet, commonly gifted during celebrations like Diwali. I got this recipe from my neighbor when I lived in India. She always brought me sweets that she made herself."</t>
   </si>
   <si>
@@ -1304,11 +1145,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -1318,20 +1165,9 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
     </font>
     <font>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1380,15 +1216,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1396,20 +1232,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1626,31 +1459,34 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="9" width="7.63"/>
-    <col customWidth="1" min="10" max="10" width="14.5"/>
-    <col customWidth="1" min="11" max="11" width="17.88"/>
+    <col customWidth="1" min="1" max="1" width="20.5"/>
+    <col customWidth="1" min="2" max="2" width="20.13"/>
+    <col customWidth="1" min="3" max="3" width="21.5"/>
+    <col customWidth="1" min="4" max="7" width="7.63"/>
+    <col customWidth="1" min="8" max="8" width="14.5"/>
+    <col customWidth="1" min="9" max="9" width="17.88"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1659,1772 +1495,1466 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>21</v>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>21</v>
+      <c r="I4" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>21</v>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>21</v>
+        <v>38</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>87</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>21</v>
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>87</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>21</v>
+        <v>88</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>21</v>
+        <v>93</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>21</v>
+        <v>98</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>21</v>
+        <v>103</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>21</v>
+        <v>108</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>21</v>
+        <v>119</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>21</v>
+        <v>125</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>21</v>
+        <v>131</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>21</v>
+        <v>136</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>21</v>
+        <v>142</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>21</v>
+        <v>148</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>87</v>
+        <v>153</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>21</v>
+      <c r="A27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>21</v>
+        <v>164</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>21</v>
+        <v>169</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>21</v>
+        <v>174</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>21</v>
+        <v>179</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K32" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>87</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>21</v>
+        <v>190</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>21</v>
+        <v>196</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>21</v>
+        <v>201</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>21</v>
+        <v>207</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>87</v>
+        <v>212</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>21</v>
+        <v>218</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>21</v>
+        <v>223</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>21</v>
+        <v>229</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>21</v>
+        <v>234</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>21</v>
+        <v>240</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>21</v>
+        <v>245</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K44" s="8" t="s">
-        <v>21</v>
+        <v>251</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>303</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>21</v>
+        <v>257</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>21</v>
+        <v>262</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>21</v>
+        <v>267</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="L48" s="8" t="s">
-        <v>328</v>
+        <v>272</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="I48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>332</v>
+      <c r="A49" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>283</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>328</v>
+        <v>284</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>339</v>
+      <c r="A50" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>289</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>328</v>
+        <v>290</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H50" s="5"/>
+      <c r="I50" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J50" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>328</v>
+      <c r="A51" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="I51" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="J52" s="6"/>
+      <c r="H52" s="5"/>
     </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
@@ -4376,107 +3906,60 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink r:id="rId2" ref="E3"/>
-    <hyperlink r:id="rId3" ref="E4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="E5"/>
-    <hyperlink r:id="rId6" ref="B6"/>
-    <hyperlink r:id="rId7" ref="E6"/>
-    <hyperlink r:id="rId8" ref="B7"/>
-    <hyperlink r:id="rId9" ref="E7"/>
-    <hyperlink r:id="rId10" ref="B8"/>
-    <hyperlink r:id="rId11" ref="E8"/>
-    <hyperlink r:id="rId12" ref="B9"/>
-    <hyperlink r:id="rId13" ref="E9"/>
-    <hyperlink r:id="rId14" ref="B10"/>
-    <hyperlink r:id="rId15" ref="E10"/>
-    <hyperlink r:id="rId16" ref="B11"/>
-    <hyperlink r:id="rId17" ref="E11"/>
-    <hyperlink r:id="rId18" ref="B12"/>
-    <hyperlink r:id="rId19" ref="E12"/>
-    <hyperlink r:id="rId20" ref="B13"/>
-    <hyperlink r:id="rId21" ref="E13"/>
-    <hyperlink r:id="rId22" ref="B14"/>
-    <hyperlink r:id="rId23" ref="E14"/>
-    <hyperlink r:id="rId24" ref="B15"/>
-    <hyperlink r:id="rId25" ref="E15"/>
-    <hyperlink r:id="rId26" ref="B16"/>
-    <hyperlink r:id="rId27" ref="E16"/>
-    <hyperlink r:id="rId28" ref="B17"/>
-    <hyperlink r:id="rId29" ref="E17"/>
-    <hyperlink r:id="rId30" ref="B18"/>
-    <hyperlink r:id="rId31" ref="E18"/>
-    <hyperlink r:id="rId32" ref="B19"/>
-    <hyperlink r:id="rId33" ref="E19"/>
-    <hyperlink r:id="rId34" ref="B20"/>
-    <hyperlink r:id="rId35" ref="E20"/>
-    <hyperlink r:id="rId36" ref="B21"/>
-    <hyperlink r:id="rId37" ref="E21"/>
-    <hyperlink r:id="rId38" ref="B22"/>
-    <hyperlink r:id="rId39" ref="E22"/>
-    <hyperlink r:id="rId40" ref="B23"/>
-    <hyperlink r:id="rId41" ref="E23"/>
-    <hyperlink r:id="rId42" ref="B24"/>
-    <hyperlink r:id="rId43" ref="E24"/>
-    <hyperlink r:id="rId44" ref="B25"/>
-    <hyperlink r:id="rId45" ref="E25"/>
-    <hyperlink r:id="rId46" ref="B26"/>
-    <hyperlink r:id="rId47" ref="E26"/>
-    <hyperlink r:id="rId48" ref="B27"/>
-    <hyperlink r:id="rId49" ref="E27"/>
-    <hyperlink r:id="rId50" ref="B28"/>
-    <hyperlink r:id="rId51" ref="E28"/>
-    <hyperlink r:id="rId52" ref="B29"/>
-    <hyperlink r:id="rId53" ref="E29"/>
-    <hyperlink r:id="rId54" ref="B30"/>
-    <hyperlink r:id="rId55" ref="E30"/>
-    <hyperlink r:id="rId56" ref="B31"/>
-    <hyperlink r:id="rId57" ref="E31"/>
-    <hyperlink r:id="rId58" ref="B32"/>
-    <hyperlink r:id="rId59" ref="E32"/>
-    <hyperlink r:id="rId60" ref="B33"/>
-    <hyperlink r:id="rId61" ref="E33"/>
-    <hyperlink r:id="rId62" ref="B34"/>
-    <hyperlink r:id="rId63" ref="E34"/>
-    <hyperlink r:id="rId64" ref="B35"/>
-    <hyperlink r:id="rId65" ref="E35"/>
-    <hyperlink r:id="rId66" ref="B36"/>
-    <hyperlink r:id="rId67" ref="E36"/>
-    <hyperlink r:id="rId68" ref="B37"/>
-    <hyperlink r:id="rId69" ref="E37"/>
-    <hyperlink r:id="rId70" ref="B38"/>
-    <hyperlink r:id="rId71" ref="E38"/>
-    <hyperlink r:id="rId72" ref="B39"/>
-    <hyperlink r:id="rId73" ref="E39"/>
-    <hyperlink r:id="rId74" ref="B40"/>
-    <hyperlink r:id="rId75" ref="E40"/>
-    <hyperlink r:id="rId76" ref="B41"/>
-    <hyperlink r:id="rId77" ref="E41"/>
-    <hyperlink r:id="rId78" ref="B42"/>
-    <hyperlink r:id="rId79" ref="E42"/>
-    <hyperlink r:id="rId80" ref="B43"/>
-    <hyperlink r:id="rId81" ref="E43"/>
-    <hyperlink r:id="rId82" ref="B44"/>
-    <hyperlink r:id="rId83" ref="E44"/>
-    <hyperlink r:id="rId84" ref="B45"/>
-    <hyperlink r:id="rId85" ref="E45"/>
-    <hyperlink r:id="rId86" ref="B46"/>
-    <hyperlink r:id="rId87" ref="E46"/>
-    <hyperlink r:id="rId88" ref="B47"/>
-    <hyperlink r:id="rId89" ref="E47"/>
-    <hyperlink r:id="rId90" ref="B48"/>
-    <hyperlink r:id="rId91" ref="E48"/>
-    <hyperlink r:id="rId92" ref="B49"/>
-    <hyperlink r:id="rId93" ref="E49"/>
-    <hyperlink r:id="rId94" ref="B50"/>
-    <hyperlink r:id="rId95" ref="E50"/>
-    <hyperlink r:id="rId96" ref="B51"/>
-    <hyperlink r:id="rId97" ref="E51"/>
+    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
+    <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId5" ref="C6"/>
+    <hyperlink r:id="rId6" ref="C7"/>
+    <hyperlink r:id="rId7" ref="C8"/>
+    <hyperlink r:id="rId8" ref="C9"/>
+    <hyperlink r:id="rId9" ref="C10"/>
+    <hyperlink r:id="rId10" ref="C11"/>
+    <hyperlink r:id="rId11" ref="C12"/>
+    <hyperlink r:id="rId12" ref="C13"/>
+    <hyperlink r:id="rId13" ref="C14"/>
+    <hyperlink r:id="rId14" ref="C15"/>
+    <hyperlink r:id="rId15" ref="C16"/>
+    <hyperlink r:id="rId16" ref="C17"/>
+    <hyperlink r:id="rId17" ref="C18"/>
+    <hyperlink r:id="rId18" ref="C19"/>
+    <hyperlink r:id="rId19" ref="C20"/>
+    <hyperlink r:id="rId20" ref="C21"/>
+    <hyperlink r:id="rId21" ref="C22"/>
+    <hyperlink r:id="rId22" ref="C23"/>
+    <hyperlink r:id="rId23" ref="C24"/>
+    <hyperlink r:id="rId24" ref="C25"/>
+    <hyperlink r:id="rId25" ref="C26"/>
+    <hyperlink r:id="rId26" ref="C27"/>
+    <hyperlink r:id="rId27" ref="C28"/>
+    <hyperlink r:id="rId28" ref="C29"/>
+    <hyperlink r:id="rId29" ref="C30"/>
+    <hyperlink r:id="rId30" ref="C31"/>
+    <hyperlink r:id="rId31" ref="C32"/>
+    <hyperlink r:id="rId32" ref="C33"/>
+    <hyperlink r:id="rId33" ref="C34"/>
+    <hyperlink r:id="rId34" ref="C35"/>
+    <hyperlink r:id="rId35" ref="C36"/>
+    <hyperlink r:id="rId36" ref="C37"/>
+    <hyperlink r:id="rId37" ref="C38"/>
+    <hyperlink r:id="rId38" ref="C39"/>
+    <hyperlink r:id="rId39" ref="C40"/>
+    <hyperlink r:id="rId40" ref="C41"/>
+    <hyperlink r:id="rId41" ref="C42"/>
+    <hyperlink r:id="rId42" ref="C43"/>
+    <hyperlink r:id="rId43" ref="C44"/>
+    <hyperlink r:id="rId44" ref="C45"/>
+    <hyperlink r:id="rId45" ref="C46"/>
+    <hyperlink r:id="rId46" ref="C47"/>
+    <hyperlink r:id="rId47" ref="C48"/>
+    <hyperlink r:id="rId48" ref="C49"/>
+    <hyperlink r:id="rId49" ref="C50"/>
+    <hyperlink r:id="rId50" ref="C51"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId98"/>
+  <drawing r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>